<commit_message>
commited by globy on 15 june
</commit_message>
<xml_diff>
--- a/7rmartSupermarket/src/main/java/Resources/TestData.xlsx
+++ b/7rmartSupermarket/src/main/java/Resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19770" windowHeight="6615" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15555" windowHeight="2850"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L13"/>
+  <oleSize ref="A1:P14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>admin</t>
   </si>
@@ -47,16 +47,37 @@
   </si>
   <si>
     <t>GY1</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>google</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -79,13 +100,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,31 +409,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -417,7 +447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -427,6 +457,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -434,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>